<commit_message>
latest work cleaning pipeline
</commit_message>
<xml_diff>
--- a/src/data/inputs/entsog_points_mapping.xlsx
+++ b/src/data/inputs/entsog_points_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/bruegel/data_new/WORKING/ENERGY/gas-demand/src/data/inputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9640236A-5E79-5549-BF71-4A8E90D7D027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{435B21C3-EE8B-224F-9D96-5A0E3374AD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27460" windowHeight="19660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -735,8 +735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H996"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="138" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="138" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>